<commit_message>
add user script for UX
add user script for UX
</commit_message>
<xml_diff>
--- a/Status Reports/10-28-2023 Status Report.xlsx
+++ b/Status Reports/10-28-2023 Status Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianja\OneDrive\Documents\Fall 2023 Semester\CS 428\Status Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nobib\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5995D6-816E-4D6D-A7AD-1E87A4A36E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64160A95-76A5-4D79-9B17-985C7466502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status Report" sheetId="1" r:id="rId1"/>
@@ -646,6 +646,193 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -658,215 +845,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -969,6 +955,20 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,117 +1282,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="77" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78">
+      <c r="G1" s="12"/>
+      <c r="H1" s="13">
         <v>45227</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="77" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="76" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="69" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="71"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="74" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="9"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="74" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="79" t="s">
+      <c r="K4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="43"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="74" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="3">
         <v>1</v>
       </c>
@@ -1400,21 +1400,21 @@
         <v>13</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="43"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="74" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="3">
         <v>0.1</v>
       </c>
@@ -1422,21 +1422,21 @@
         <v>11</v>
       </c>
       <c r="L6" s="9"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="43"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="25"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="74" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="3">
         <v>0.1</v>
       </c>
@@ -1444,19 +1444,19 @@
         <v>11</v>
       </c>
       <c r="L7" s="9"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="43"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="3">
         <v>0</v>
       </c>
@@ -1464,19 +1464,19 @@
         <v>14</v>
       </c>
       <c r="L8" s="9"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="43"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="25"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="3">
         <v>0</v>
       </c>
@@ -1484,19 +1484,19 @@
         <v>14</v>
       </c>
       <c r="L9" s="9"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="43"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="25"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="64"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="4">
         <v>0</v>
       </c>
@@ -1504,374 +1504,411 @@
         <v>14</v>
       </c>
       <c r="L10" s="9"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="52"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="36"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48" t="s">
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="31"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="58" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58" t="s">
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="60"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="44"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="55"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="60"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="60"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="44"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="60"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="62"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="76"/>
+      <c r="C18" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="46"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="78"/>
       <c r="E19" s="5">
         <v>6</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="29"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="68"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="5">
         <v>2</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="32"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="71"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15" t="s">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="5">
         <v>3</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="35"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="74"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="5">
-        <v>4</v>
-      </c>
-      <c r="F22" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="29"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="68"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="40" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="5">
         <v>3.5</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="32"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="71"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="35"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="74"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="20"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="59"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="23"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="62"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="26"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="65"/>
     </row>
     <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
       <c r="E28" s="7">
         <f>SUM(E19:E27)</f>
-        <v>18.5</v>
-      </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="38"/>
+        <v>19.5</v>
+      </c>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G25:N27"/>
+    <mergeCell ref="G22:N24"/>
+    <mergeCell ref="G19:N21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="F28:N28"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G18:N18"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="A12:E16"/>
+    <mergeCell ref="F12:I16"/>
+    <mergeCell ref="J12:N16"/>
+    <mergeCell ref="A3:F10"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="K2:L2"/>
@@ -1888,49 +1925,12 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="G18:N18"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="F17:N17"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="A12:E16"/>
-    <mergeCell ref="F12:I16"/>
-    <mergeCell ref="J12:N16"/>
-    <mergeCell ref="A3:F10"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="F28:N28"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G25:N27"/>
-    <mergeCell ref="G22:N24"/>
-    <mergeCell ref="G19:N21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="E19:E22">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
@@ -1940,66 +1940,66 @@
       <formula>252250</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Delayed">
+      <formula>NOT(ISERROR(SEARCH("Delayed",K5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="delays">
+      <formula>NOT(ISERROR(SEARCH("delays",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K3:L10">
-    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="Track">
+    <cfRule type="containsText" dxfId="14" priority="24" operator="containsText" text="Track">
       <formula>NOT(ISERROR(SEARCH("Track",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="26" operator="containsText" text="Ontrack">
+    <cfRule type="containsText" dxfId="12" priority="26" operator="containsText" text="Ontrack">
       <formula>NOT(ISERROR(SEARCH("Ontrack",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="Delayed">
+    <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="Delayed">
       <formula>NOT(ISERROR(SEARCH("Delayed",K4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="delays">
+    <cfRule type="containsText" dxfId="10" priority="23" operator="containsText" text="delays">
       <formula>NOT(ISERROR(SEARCH("delays",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:L5">
-    <cfRule type="containsText" dxfId="11" priority="20" operator="containsText" text="Possible">
+    <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="Possible">
       <formula>NOT(ISERROR(SEARCH("Possible",K5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="21" operator="containsText" text="delay">
+    <cfRule type="containsText" dxfId="8" priority="21" operator="containsText" text="delay">
       <formula>NOT(ISERROR(SEARCH("delay",K5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="22" operator="containsText" text="complete">
+    <cfRule type="containsText" dxfId="7" priority="22" operator="containsText" text="complete">
       <formula>NOT(ISERROR(SEARCH("complete",K5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6">
-    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="18" operator="containsText" text="Delays">
+    <cfRule type="containsText" dxfId="5" priority="18" operator="containsText" text="Delays">
       <formula>NOT(ISERROR(SEARCH("Delays",K6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:L8">
-    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="Delayed">
+    <cfRule type="containsText" dxfId="4" priority="15" operator="containsText" text="Delayed">
       <formula>NOT(ISERROR(SEARCH("Delayed",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text="delays">
+    <cfRule type="containsText" dxfId="3" priority="16" operator="containsText" text="delays">
       <formula>NOT(ISERROR(SEARCH("delays",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:L9">
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="Possible">
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="Possible">
       <formula>NOT(ISERROR(SEARCH("Possible",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="delay">
+    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="delay">
       <formula>NOT(ISERROR(SEARCH("delay",K9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="complete">
+    <cfRule type="containsText" dxfId="0" priority="14" operator="containsText" text="complete">
       <formula>NOT(ISERROR(SEARCH("complete",K9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Delayed">
-      <formula>NOT(ISERROR(SEARCH("Delayed",K5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="delays">
-      <formula>NOT(ISERROR(SEARCH("delays",K5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>